<commit_message>
Prevented below-zero figures from showing.
</commit_message>
<xml_diff>
--- a/data/mapdata_india_sanitation_districts_2.xlsx
+++ b/data/mapdata_india_sanitation_districts_2.xlsx
@@ -3710,7 +3710,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3727,6 +3727,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3758,7 +3764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3773,6 +3779,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4077,8 +4088,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH647"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A627" workbookViewId="0">
-      <selection activeCell="A641" sqref="A641"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A355" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I370" sqref="I370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43228,90 +43240,89 @@
         <v>581.99842999999998</v>
       </c>
     </row>
-    <row r="483" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A483" s="3" t="s">
+    <row r="483" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A483" s="8" t="s">
         <v>904</v>
       </c>
-      <c r="B483" s="2" t="s">
+      <c r="B483" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="C483" s="7"/>
-      <c r="G483">
+      <c r="G483" s="10">
         <v>10.715425491333008</v>
       </c>
-      <c r="H483">
+      <c r="H483" s="10">
         <v>0.26599245071411132</v>
       </c>
-      <c r="I483">
+      <c r="I483" s="10">
         <v>82.426346406455238</v>
       </c>
-      <c r="J483">
+      <c r="J483" s="10">
         <v>-0.57563581349537285</v>
       </c>
-      <c r="K483">
+      <c r="K483" s="10">
         <v>13.375349998474121</v>
       </c>
-      <c r="L483">
+      <c r="L483" s="10">
         <v>76.669988271501509</v>
       </c>
-      <c r="M483">
+      <c r="M483" s="10">
         <v>-3.6098299503326414</v>
       </c>
-      <c r="N483">
+      <c r="N483" s="10">
         <v>-18.591861254380003</v>
       </c>
-      <c r="P483">
+      <c r="P483" s="10">
         <v>1.8964259664478482</v>
       </c>
-      <c r="Q483">
+      <c r="Q483" s="10">
         <v>26</v>
       </c>
-      <c r="R483">
+      <c r="R483" s="10">
         <v>910000</v>
       </c>
-      <c r="S483">
+      <c r="S483" s="10">
         <v>9.1</v>
       </c>
-      <c r="T483">
+      <c r="T483" s="10">
         <v>22.121896162528216</v>
       </c>
-      <c r="U483">
+      <c r="U483" s="10">
         <v>98</v>
       </c>
-      <c r="V483">
+      <c r="V483" s="10">
         <v>784000</v>
       </c>
-      <c r="W483">
+      <c r="W483" s="10">
         <v>7.84</v>
       </c>
-      <c r="X483">
+      <c r="X483" s="10">
         <v>131</v>
       </c>
-      <c r="Y483">
+      <c r="Y483" s="10">
         <v>26200000</v>
       </c>
-      <c r="Z483">
+      <c r="Z483" s="10">
         <v>262</v>
       </c>
-      <c r="AA483">
+      <c r="AA483" s="10">
         <v>37.079241814617859</v>
       </c>
-      <c r="AB483">
+      <c r="AB483" s="10">
         <v>54416</v>
       </c>
-      <c r="AC483">
+      <c r="AC483" s="10">
         <v>593134400</v>
       </c>
-      <c r="AD483">
+      <c r="AD483" s="10">
         <v>5931.3440000000001</v>
       </c>
-      <c r="AE483">
+      <c r="AE483" s="10">
         <v>621028400</v>
       </c>
-      <c r="AF483">
+      <c r="AF483" s="10">
         <v>6210.2839999999997</v>
       </c>
-      <c r="AG483">
+      <c r="AG483" s="10">
         <v>62.102839999999993</v>
       </c>
     </row>

</xml_diff>